<commit_message>
Added Check for engineering units on analogs
</commit_message>
<xml_diff>
--- a/dist/Attachment 3-Attribute Names & Engineering Units.xlsx
+++ b/dist/Attachment 3-Attribute Names & Engineering Units.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://clearwayenergy.sharepoint.com/sites/OperationsIT/Standards/Utility/EPC Exhibit A-11 Package 3.0/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matthew.Bogucki\PycharmProjects\PointsListValidator\dist\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="656" documentId="13_ncr:1_{4BD359D7-C9DB-4D4F-881C-1F9AC5E9D2AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{01373C0E-C8DA-4177-AED8-5040612C0D70}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{463C8533-103D-4E67-9D14-71F196980E9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="728" firstSheet="3" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="728" firstSheet="8" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TagNaming Criteria and Examples" sheetId="12" r:id="rId1"/>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2084" uniqueCount="500">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2087" uniqueCount="500">
   <si>
     <t>Point Names follow the naming convention:</t>
   </si>
@@ -1954,7 +1954,17 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
-  <dxfs count="40">
+  <dxfs count="41">
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C5700"/>
@@ -4009,7 +4019,7 @@
   </sheetData>
   <phoneticPr fontId="7" type="noConversion"/>
   <conditionalFormatting sqref="A1">
-    <cfRule type="duplicateValues" dxfId="11" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="12" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -4291,7 +4301,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1">
-    <cfRule type="duplicateValues" dxfId="10" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="11" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="240" verticalDpi="240" r:id="rId1"/>
@@ -4302,7 +4312,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:J67"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
@@ -5166,7 +5176,7 @@
   </sheetData>
   <autoFilter ref="A1:E38" xr:uid="{270E9F6F-3E54-4333-8639-E0503346C70D}"/>
   <conditionalFormatting sqref="A1">
-    <cfRule type="duplicateValues" dxfId="9" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="10" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="240" verticalDpi="240" r:id="rId1"/>
@@ -5728,7 +5738,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1">
-    <cfRule type="duplicateValues" dxfId="8" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="9" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5782,10 +5792,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2">
-    <cfRule type="duplicateValues" dxfId="7" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="8" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1">
-    <cfRule type="duplicateValues" dxfId="6" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5844,10 +5854,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2">
-    <cfRule type="duplicateValues" dxfId="5" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1">
-    <cfRule type="duplicateValues" dxfId="4" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5906,10 +5916,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2">
-    <cfRule type="duplicateValues" dxfId="3" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1">
-    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5919,8 +5929,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -5928,7 +5938,7 @@
     <col min="1" max="1" width="28.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="30.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="30.140625" customWidth="1"/>
-    <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="48.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -5959,6 +5969,9 @@
       <c r="C2" t="s">
         <v>83</v>
       </c>
+      <c r="D2" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -5970,6 +5983,9 @@
       <c r="C3" t="s">
         <v>118</v>
       </c>
+      <c r="D3" t="s">
+        <v>432</v>
+      </c>
       <c r="E3" t="s">
         <v>433</v>
       </c>
@@ -5984,12 +6000,18 @@
       <c r="C4" t="s">
         <v>118</v>
       </c>
+      <c r="D4" t="s">
+        <v>434</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A4:A1048576 E2">
+    <cfRule type="duplicateValues" dxfId="2" priority="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1">
     <cfRule type="duplicateValues" dxfId="1" priority="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1">
+  <conditionalFormatting sqref="D4">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6769,16 +6791,16 @@
   </sheetData>
   <phoneticPr fontId="7" type="noConversion"/>
   <conditionalFormatting sqref="D10:D13">
-    <cfRule type="duplicateValues" dxfId="39" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="40" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A10:A19 A2:A5 A7 A23:A51">
-    <cfRule type="duplicateValues" dxfId="38" priority="19"/>
+    <cfRule type="duplicateValues" dxfId="39" priority="19"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A8:A9">
-    <cfRule type="duplicateValues" dxfId="37" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="38" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1">
-    <cfRule type="duplicateValues" dxfId="36" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="37" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="240" verticalDpi="240" r:id="rId1"/>
@@ -7017,31 +7039,31 @@
   </sheetData>
   <autoFilter ref="A1:B91" xr:uid="{AE146147-637B-4DFF-B80F-70F650457718}"/>
   <conditionalFormatting sqref="A16:A1048576 A1">
-    <cfRule type="duplicateValues" dxfId="35" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="36" priority="11"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A10:A12 A14:A15">
-    <cfRule type="duplicateValues" dxfId="34" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="35" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A13">
-    <cfRule type="duplicateValues" dxfId="33" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="34" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D10:D12 D14:D15">
-    <cfRule type="duplicateValues" dxfId="32" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="33" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D13">
-    <cfRule type="duplicateValues" dxfId="31" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="32" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:A8">
-    <cfRule type="duplicateValues" dxfId="30" priority="52"/>
+    <cfRule type="duplicateValues" dxfId="31" priority="52"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D8">
-    <cfRule type="duplicateValues" dxfId="29" priority="54"/>
+    <cfRule type="duplicateValues" dxfId="30" priority="54"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A9">
-    <cfRule type="duplicateValues" dxfId="28" priority="56"/>
+    <cfRule type="duplicateValues" dxfId="29" priority="56"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D9">
-    <cfRule type="duplicateValues" dxfId="27" priority="58"/>
+    <cfRule type="duplicateValues" dxfId="28" priority="58"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="240" verticalDpi="240" r:id="rId1"/>
@@ -8065,7 +8087,7 @@
   <autoFilter ref="A1:E69" xr:uid="{30DB61DF-688D-497A-8341-91EC4194A25F}"/>
   <phoneticPr fontId="7" type="noConversion"/>
   <conditionalFormatting sqref="A1">
-    <cfRule type="duplicateValues" dxfId="26" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="27" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -8712,10 +8734,10 @@
   </sheetData>
   <autoFilter ref="A1:E64" xr:uid="{30DB61DF-688D-497A-8341-91EC4194A25F}"/>
   <conditionalFormatting sqref="A1">
-    <cfRule type="duplicateValues" dxfId="25" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="26" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="duplicateValues" dxfId="24" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="25" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -9386,10 +9408,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:A4">
-    <cfRule type="duplicateValues" dxfId="23" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="24" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1">
-    <cfRule type="duplicateValues" dxfId="22" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="23" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="240" r:id="rId1"/>
@@ -9553,13 +9575,13 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:A4">
-    <cfRule type="duplicateValues" dxfId="21" priority="15"/>
+    <cfRule type="duplicateValues" dxfId="22" priority="15"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A6">
-    <cfRule type="duplicateValues" dxfId="20" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="21" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1">
-    <cfRule type="duplicateValues" dxfId="19" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="20" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -10232,13 +10254,13 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:A4 A6:A13 A17:A45">
-    <cfRule type="duplicateValues" dxfId="18" priority="17"/>
+    <cfRule type="duplicateValues" dxfId="19" priority="17"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6">
-    <cfRule type="duplicateValues" dxfId="17" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="18" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1">
-    <cfRule type="duplicateValues" dxfId="16" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="17" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -10729,34 +10751,34 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D6:D8">
-    <cfRule type="duplicateValues" dxfId="15" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="16" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D9">
-    <cfRule type="duplicateValues" dxfId="14" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="15" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1">
-    <cfRule type="duplicateValues" dxfId="13" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="14" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A11:A16 A2:A4 A6:A9 A20:A32">
-    <cfRule type="duplicateValues" dxfId="12" priority="59"/>
+    <cfRule type="duplicateValues" dxfId="13" priority="59"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -10957,18 +10979,18 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6D96781B-1881-445E-8910-97FFAA6E87E1}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B36C8ED1-9097-42B4-96C5-752170CF076E}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B36C8ED1-9097-42B4-96C5-752170CF076E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6D96781B-1881-445E-8910-97FFAA6E87E1}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>